<commit_message>
set up esp idf, vscode, and the start program.
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\dashcam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\dashcam\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E032874-A116-42C1-9CDC-EE960956C52F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A3BB1-7AF4-42ED-B907-14EE7F457A33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Outline" sheetId="7" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
   <si>
     <t>Risk</t>
   </si>
@@ -396,12 +396,6 @@
     <t>LEDs</t>
   </si>
   <si>
-    <t>Access SD card</t>
-  </si>
-  <si>
-    <t>ESP32-CAM</t>
-  </si>
-  <si>
     <t>LEDS</t>
   </si>
   <si>
@@ -411,12 +405,6 @@
     <t>Structure for plan- will use excel sheet, gantt charts</t>
   </si>
   <si>
-    <t>ESP32 video capture</t>
-  </si>
-  <si>
-    <t>ESP32 access SD card</t>
-  </si>
-  <si>
     <t>ESP32 save video to SD card</t>
   </si>
   <si>
@@ -472,6 +460,24 @@
   </si>
   <si>
     <t>DASHCAM</t>
+  </si>
+  <si>
+    <t>SD card research</t>
+  </si>
+  <si>
+    <t>ESP32 SD card research</t>
+  </si>
+  <si>
+    <t>ESP32-cam development env setup</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>ESP32-CAM on pcb</t>
   </si>
 </sst>
 </file>
@@ -1761,7 +1767,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -1799,7 +1805,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
@@ -1936,8 +1942,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1959,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="47" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="1"/>
@@ -2136,7 +2142,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2225,19 +2231,25 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="36">
+        <v>44310</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2248,6 +2260,9 @@
       <c r="D16">
         <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -2267,6 +2282,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
@@ -2285,6 +2303,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
       <c r="G18" t="s">
         <v>14</v>
       </c>
@@ -2309,13 +2330,16 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
       <c r="G20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -2325,6 +2349,9 @@
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="G21" t="s">
@@ -2345,6 +2372,9 @@
         <f>IFERROR(INDEX($J$3:$L$5,MATCH(C22,$J$2:$L$2,0),MATCH(B22,$I$3:$I$5,0)),"")</f>
         <v>21</v>
       </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
@@ -2363,6 +2393,9 @@
         <f>IFERROR(INDEX($J$3:$L$5,MATCH(C23,$J$2:$L$2,0),MATCH(B23,$I$3:$I$5,0)),"")</f>
         <v>21</v>
       </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
@@ -2381,6 +2414,9 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="E24" t="s">
+        <v>112</v>
+      </c>
       <c r="G24" t="s">
         <v>14</v>
       </c>
@@ -2411,13 +2447,16 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
       <c r="G27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -2427,6 +2466,9 @@
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
         <v>5</v>
       </c>
       <c r="G28" t="s">
@@ -2447,6 +2489,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
       <c r="G29" t="s">
         <v>14</v>
       </c>
@@ -2465,6 +2510,9 @@
         <f>IFERROR(INDEX($J$3:$L$5,MATCH(C30,$J$2:$L$2,0),MATCH(B30,$I$3:$I$5,0)),"")</f>
         <v>5</v>
       </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
       <c r="G30" t="s">
         <v>14</v>
       </c>
@@ -2483,6 +2531,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
       <c r="G31" t="s">
         <v>14</v>
       </c>
@@ -2501,6 +2552,9 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
       <c r="G32" t="s">
         <v>14</v>
       </c>
@@ -2525,6 +2579,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E34" t="s">
+        <v>113</v>
+      </c>
       <c r="G34" t="s">
         <v>14</v>
       </c>
@@ -2543,6 +2600,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E35" t="s">
+        <v>113</v>
+      </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
@@ -2561,7 +2621,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -2573,13 +2633,16 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
       <c r="G38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -2590,6 +2653,9 @@
       <c r="D39">
         <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
@@ -2609,6 +2675,9 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
       <c r="G40" t="s">
         <v>14</v>
       </c>
@@ -2627,13 +2696,16 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
       <c r="G41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -2645,6 +2717,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
       <c r="G42" t="s">
         <v>14</v>
       </c>
@@ -2657,7 +2732,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -2668,6 +2743,9 @@
       <c r="D44">
         <f t="shared" si="0"/>
         <v>55</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
       </c>
       <c r="G44" t="s">
         <v>14</v>
@@ -2863,7 +2941,7 @@
       <formula>NOT(ISERROR(SEARCH("Ongoing",O6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E1048576 E25:E28 E22:E23 H10 E1:E19">
+  <conditionalFormatting sqref="E1:E1048576 H10">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2887,8 +2965,8 @@
   </sheetPr>
   <dimension ref="A1:BO33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2983,7 +3061,7 @@
     <row r="2" spans="1:67" s="9" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
       <c r="B2" s="51" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -3791,22 +3869,22 @@
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B9" s="38" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C9" s="39">
         <v>1</v>
       </c>
       <c r="D9" s="39">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E9" s="39">
         <v>1</v>
       </c>
-      <c r="F9" s="39" t="s">
-        <v>37</v>
+      <c r="F9" s="39">
+        <v>0.3</v>
       </c>
       <c r="G9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -3871,7 +3949,7 @@
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B10" s="38" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C10" s="39">
         <v>2</v>
@@ -3879,8 +3957,8 @@
       <c r="D10" s="39">
         <v>0.5</v>
       </c>
-      <c r="E10" s="39" t="s">
-        <v>37</v>
+      <c r="E10" s="39">
+        <v>1</v>
       </c>
       <c r="F10" s="39" t="s">
         <v>37</v>
@@ -3951,7 +4029,7 @@
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B11" s="38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" s="39">
         <v>2</v>
@@ -4031,7 +4109,7 @@
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B12" s="38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C12" s="39">
         <v>3</v>
@@ -4111,7 +4189,7 @@
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B13" s="38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C13" s="39">
         <v>3</v>
@@ -4265,7 +4343,7 @@
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B15" s="38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C15" s="39">
         <v>5</v>
@@ -4345,7 +4423,7 @@
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B16" s="38" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C16" s="39">
         <v>6</v>
@@ -4425,7 +4503,7 @@
     </row>
     <row r="17" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B17" s="38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C17" s="39">
         <v>6</v>
@@ -4585,7 +4663,7 @@
     </row>
     <row r="19" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B19" s="38" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C19" s="39">
         <v>7</v>
@@ -4665,7 +4743,7 @@
     </row>
     <row r="20" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B20" s="38" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C20" s="39">
         <v>7</v>
@@ -4739,7 +4817,7 @@
     </row>
     <row r="21" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B21" s="38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C21" s="39">
         <v>8</v>
@@ -4819,7 +4897,7 @@
     </row>
     <row r="22" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B22" s="38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C22" s="39">
         <v>10</v>
@@ -4899,7 +4977,7 @@
     </row>
     <row r="23" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B23" s="38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C23" s="39">
         <v>10</v>
@@ -4979,7 +5057,7 @@
     </row>
     <row r="24" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B24" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="39">
         <v>11</v>
@@ -5059,7 +5137,7 @@
     </row>
     <row r="25" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B25" s="38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C25" s="39">
         <v>13</v>
@@ -5139,7 +5217,7 @@
     </row>
     <row r="26" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B26" s="38" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C26" s="39">
         <v>15</v>

</xml_diff>

<commit_message>
add 128x32 oled to schem. add new symbols to library. add backup power (supercap) circuit. update plan. add esp32 pinouts
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BB504F-4072-4093-8BF3-1DA36A316E56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435A7AD9-E6E9-42A5-A4A9-63D185AF45AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Outline" sheetId="7" r:id="rId1"/>
     <sheet name="Project Task Overview" sheetId="1" r:id="rId2"/>
     <sheet name="Gantt Chart" sheetId="6" r:id="rId3"/>
+    <sheet name="Daily Notes" sheetId="8" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="Actual" localSheetId="2">('Gantt Chart'!PeriodInActual*('Gantt Chart'!$E1&gt;0))*'Gantt Chart'!PeriodInPlan</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="191">
   <si>
     <t>Risk</t>
   </si>
@@ -351,21 +352,12 @@
     <t>Select Battery</t>
   </si>
   <si>
-    <t>Select charge IC</t>
-  </si>
-  <si>
-    <t>Select safety IC</t>
-  </si>
-  <si>
     <t>Record video instantly when turned on</t>
   </si>
   <si>
     <t>SD card to store videos, delete oldest video (not included in cost)</t>
   </si>
   <si>
-    <t>Develop battery charge prototype</t>
-  </si>
-  <si>
     <t>Product block diagram</t>
   </si>
   <si>
@@ -411,12 +403,6 @@
     <t>Bluetooth ESP32 research</t>
   </si>
   <si>
-    <t>Design battery protection</t>
-  </si>
-  <si>
-    <t>Test battery charge prototype</t>
-  </si>
-  <si>
     <t>Test buttons</t>
   </si>
   <si>
@@ -426,9 +412,6 @@
     <t>Bluetooth research on ESP32</t>
   </si>
   <si>
-    <t>Order parts for battery charger</t>
-  </si>
-  <si>
     <t>Mechanical</t>
   </si>
   <si>
@@ -525,12 +508,6 @@
     <t>Testing SSD1306, I2C, 128x32 OLED screen</t>
   </si>
   <si>
-    <t>Will use Arduino IDE for quick prototyping. Adafruit library will not work as can't swap I2C pins and the pins they use collide with camera, using u8g2 instead.</t>
-  </si>
-  <si>
-    <t>Decided on 128x32 screen with scrolling text.</t>
-  </si>
-  <si>
     <t>GPIO peripherals research</t>
   </si>
   <si>
@@ -559,6 +536,177 @@
   </si>
   <si>
     <t>Schematic Design</t>
+  </si>
+  <si>
+    <t>Test super-capacitor with a basic circuit- calculations correct?</t>
+  </si>
+  <si>
+    <t>Add battery to schematic</t>
+  </si>
+  <si>
+    <t>Finish schematic</t>
+  </si>
+  <si>
+    <t>Test battery charge prototype with full circuit</t>
+  </si>
+  <si>
+    <t>Find out time we need to safely shut down.</t>
+  </si>
+  <si>
+    <t>Add power indicator LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wired up test circuit with super capacitor. Charging with 24 ohm resistor, discharging to an LED</t>
+  </si>
+  <si>
+    <t>Calculating time to charge isn't very accurate as when you get closer to Vsupply the current reduces, so voltage increase slows down.</t>
+  </si>
+  <si>
+    <t>Found really useful calculator to calculate charge/discharge times: http://mustcalculate.com/electronics/capacitorchargeanddischarge.php?vfrom=3.8&amp;vto=3.5&amp;vs=0&amp;c=1&amp;r=10</t>
+  </si>
+  <si>
+    <t>Realised my circuit isn't ideal- slow charge, fast discharge</t>
+  </si>
+  <si>
+    <t>Worked on coming up with a design which will charge at maximum rate (500mA) and discharge at whatever the circuit needs (max 500mA). See LTSpice simulation circuit below.</t>
+  </si>
+  <si>
+    <t>0 to 4.6V with supply voltage 4.8V, drawing 480mA (10R series resistor) = 32s</t>
+  </si>
+  <si>
+    <t>3.5V to 4.6V (with same current as above) = 19 seconds</t>
+  </si>
+  <si>
+    <t>Final thoughts:</t>
+  </si>
+  <si>
+    <t>4.6V to 3.46V (same current as above) = 2.8 seconds</t>
+  </si>
+  <si>
+    <t>Checked timing calculator, and the charging time is pretty slow, even with 500mA charge.Charging a bit more slower but having video recording on right away is better (even though turning it off less than 30 seconds will deplete battery).</t>
+  </si>
+  <si>
+    <t>LDO should work until ~3.46V</t>
+  </si>
+  <si>
+    <t>Tested Arduino script to see how quick it saves video. It's certainly less than 1 second (sent /stop command via http and I see the video gets saved less than a second).</t>
+  </si>
+  <si>
+    <t>The LCD should stay on for around 1-2 seconds to say a goodbye message, so this is plenty of tine.</t>
+  </si>
+  <si>
+    <t>ESP32 cam turns off at around 3.8V input (it's LDO has ~1V drop out as advertised)</t>
+  </si>
+  <si>
+    <t>With 5F capacitor, according to my calculations, it should take 6.7 seconds, and it takes around 7s in practice, so calculations seem accurate.</t>
+  </si>
+  <si>
+    <t>The same calculations show that 1F cap draining 200mA, to go from 4-3.5V will take over 2 seconds, which satisfies the specification.</t>
+  </si>
+  <si>
+    <t>1F cap also means the charge time will be a bit quicker.</t>
+  </si>
+  <si>
+    <t>Will use Arduino IDE for quick prototyping. Adafruit library will not work as can't swap I2C pins and the pins they use collide with camera, using u8g2 library instead.</t>
+  </si>
+  <si>
+    <t>u8g2 library works really well. Decided on 128x32 screen with scrolling text. Reason is it will have low power consumption and small size yet still displays info needed.</t>
+  </si>
+  <si>
+    <t>Dash-cams typically don't have big batteries- customers are used to plugging them in all the time (saw multiple Amazon reviews which suggest this). A supercap to safely shut down should be enough.</t>
+  </si>
+  <si>
+    <t>Why supercap? No need for over/under charge protection circuit. Can charge/discharge virtually unlimited times. Works fine in warm temperatures like inside a car (unlike NiMH). Less dangerous than Li-Ion. Takes up less space.</t>
+  </si>
+  <si>
+    <t>Supercap. Still not decided on capacitance, however will go for 5.2V+ capacitors.</t>
+  </si>
+  <si>
+    <t>Will use 1 super-capacitor (no series or parallel connection as these appear to be more risky since over-charging may happen.</t>
+  </si>
+  <si>
+    <t>Arduino script has a function which safely saves the video and shuts down. This takes less than 1 second to perform.</t>
+  </si>
+  <si>
+    <t>Notes 3</t>
+  </si>
+  <si>
+    <t>I prefer to have the circuit shut down in around 2 seconds to display a 'goodbye message'.</t>
+  </si>
+  <si>
+    <t>dV = 4.6-3.5 = 1.1</t>
+  </si>
+  <si>
+    <t>I = 0.250 A (measured 300mA peak when everything was running, so in practice it is around 250mA avg)</t>
+  </si>
+  <si>
+    <t>It = CV</t>
+  </si>
+  <si>
+    <t>It/V = C</t>
+  </si>
+  <si>
+    <t>Measuring capacitance required:</t>
+  </si>
+  <si>
+    <t>dt = 2</t>
+  </si>
+  <si>
+    <t>(0.25*2)/1.1 = 0.45F</t>
+  </si>
+  <si>
+    <t>Will Use 0.47F</t>
+  </si>
+  <si>
+    <t>According to mustcalculate.com:</t>
+  </si>
+  <si>
+    <t>Will take 36 seconds to go to full charge from empty (will take 23 seconds if charging from 3.5V)</t>
+  </si>
+  <si>
+    <t>Charging time:</t>
+  </si>
+  <si>
+    <t>Schematic checklist:</t>
+  </si>
+  <si>
+    <t>Power indicating LED</t>
+  </si>
+  <si>
+    <t>Recording LED</t>
+  </si>
+  <si>
+    <t>Button OK</t>
+  </si>
+  <si>
+    <t>Button Right</t>
+  </si>
+  <si>
+    <t>Button Left</t>
+  </si>
+  <si>
+    <t>Button ON/Off?</t>
+  </si>
+  <si>
+    <t>I2C I/O expander</t>
+  </si>
+  <si>
+    <t>Supercap</t>
+  </si>
+  <si>
+    <t>I2C OLED screen</t>
+  </si>
+  <si>
+    <t>OLED wiring:</t>
+  </si>
+  <si>
+    <t>https://www.buydisplay.com/download/ic/SSD1306.pdf</t>
+  </si>
+  <si>
+    <t>https://learn.adafruit.com/monochrome-oled-breakouts/downloads</t>
+  </si>
+  <si>
+    <t>https://www.buydisplay.com/download/interfacing/ER-OLED0.91-7_Interfacing.pdf</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1279,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1279,9 +1427,33 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1301,6 +1473,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="11" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="11" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="11" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="11" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1310,36 +1491,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="11" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="11" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="11" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="% complete" xfId="17" xr:uid="{8E59E717-42B2-4847-8690-0EA43F601F51}"/>
@@ -1601,6 +1753,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>150495</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180678</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>303459</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>77268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E77CC721-908B-44EA-90C6-0849424047E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9408795" y="4886028"/>
+          <a:ext cx="5029764" cy="3154140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>116205</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>436667</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>121093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A2DB0E2-E3B7-4DB4-ABE6-26551A143D9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9374505" y="1226820"/>
+          <a:ext cx="5197262" cy="3237673"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>267880</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>163331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{811E3D0A-E783-4857-AF1D-06083055B32F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9210675" y="8477250"/>
+          <a:ext cx="5801905" cy="3992381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>595430</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>54682</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E756B0-7A91-4DF6-AAD4-AFD7039D51EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="297180" y="9448800"/>
+          <a:ext cx="6676190" cy="4504762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1942,7 +2275,7 @@
     </row>
     <row r="5" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A5" s="44" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -1950,7 +2283,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -1988,12 +2321,12 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="45" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
@@ -2001,7 +2334,7 @@
     </row>
     <row r="20" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2028,7 +2361,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
@@ -2038,7 +2371,7 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
@@ -2121,7 +2454,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
@@ -2134,7 +2467,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="38" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
@@ -2153,68 +2486,68 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.109375" style="72" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" style="72" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="72" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" style="72"/>
+    <col min="8" max="8" width="29.109375" style="57" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" style="57" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="57" customWidth="1"/>
+    <col min="11" max="12" width="8.88671875" style="57"/>
     <col min="15" max="15" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="53"/>
+      <c r="A1" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="59"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68" t="s">
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
       <c r="O1" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="69" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="69" t="s">
+      <c r="L2" s="54" t="s">
         <v>3</v>
       </c>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54" t="s">
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="61" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2222,19 +2555,19 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="62" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="71">
+      <c r="J3" s="56">
         <v>5</v>
       </c>
-      <c r="K3" s="71">
+      <c r="K3" s="56">
         <v>13</v>
       </c>
-      <c r="L3" s="71">
+      <c r="L3" s="56">
         <v>21</v>
       </c>
       <c r="O3" t="s">
@@ -2242,25 +2575,25 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
-      <c r="H4" s="70"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="71">
+      <c r="J4" s="56">
         <v>13</v>
       </c>
-      <c r="K4" s="71">
+      <c r="K4" s="56">
         <v>21</v>
       </c>
-      <c r="L4" s="71">
+      <c r="L4" s="56">
         <v>34</v>
       </c>
       <c r="O4" t="s">
@@ -2268,25 +2601,25 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="54"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="70"/>
+      <c r="H5" s="62"/>
       <c r="I5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="56">
         <v>21</v>
       </c>
-      <c r="K5" s="71">
+      <c r="K5" s="56">
         <v>34</v>
       </c>
-      <c r="L5" s="71">
+      <c r="L5" s="56">
         <v>55</v>
       </c>
       <c r="O5" t="s">
@@ -2300,7 +2633,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2325,11 +2658,17 @@
       <c r="G8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="58" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="O8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -2355,8 +2694,8 @@
       <c r="G10" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="72" t="s">
-        <v>83</v>
+      <c r="H10" s="57" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2382,13 +2721,13 @@
       <c r="G11" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="72" t="s">
+      <c r="H11" s="57" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -2452,7 +2791,7 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F15" s="34">
         <v>44310</v>
@@ -2463,7 +2802,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2508,11 +2847,11 @@
       <c r="G17" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" s="72" t="s">
-        <v>119</v>
+      <c r="H17" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="57" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2530,7 +2869,7 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F18" s="34">
         <v>44310</v>
@@ -2538,8 +2877,8 @@
       <c r="G18" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="72" t="s">
-        <v>109</v>
+      <c r="H18" s="57" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2574,7 +2913,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -2595,7 +2934,7 @@
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2616,13 +2955,13 @@
       <c r="G22" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="72" t="s">
-        <v>111</v>
+      <c r="H22" s="57" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -2641,15 +2980,15 @@
         <v>44318</v>
       </c>
       <c r="G23" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23" s="72" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="H23" s="57" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -2662,13 +3001,13 @@
         <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F24" s="34">
         <v>44318</v>
       </c>
       <c r="G24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2679,7 +3018,7 @@
     </row>
     <row r="26" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -2692,7 +3031,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F26" s="34">
         <v>44324</v>
@@ -2700,19 +3039,19 @@
       <c r="G26" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="I26" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="J26" s="72" t="s">
-        <v>131</v>
+      <c r="H26" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="J26" s="57" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -2725,7 +3064,7 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F27" s="34">
         <v>44324</v>
@@ -2733,19 +3072,19 @@
       <c r="G27" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="72" t="s">
-        <v>133</v>
-      </c>
-      <c r="I27" s="72" t="s">
-        <v>134</v>
-      </c>
-      <c r="J27" s="72" t="s">
-        <v>135</v>
+      <c r="H27" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="J27" s="57" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -2758,7 +3097,7 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F28" s="34">
         <v>44324</v>
@@ -2766,19 +3105,19 @@
       <c r="G28" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="72" t="s">
-        <v>139</v>
-      </c>
-      <c r="I28" s="72" t="s">
-        <v>137</v>
-      </c>
-      <c r="J28" s="72" t="s">
-        <v>138</v>
+      <c r="H28" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="J28" s="57" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -2824,9 +3163,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -2845,13 +3184,19 @@
         <v>44324</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="72" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="H32" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="I32" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="J32" s="57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -2869,12 +3214,18 @@
         <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="H33" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" s="57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -2890,12 +3241,18 @@
         <v>5</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="57" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -2908,42 +3265,42 @@
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E36" t="s">
         <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D37" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -2962,9 +3319,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -2983,7 +3340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -3004,9 +3361,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -3025,9 +3382,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -3046,15 +3403,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -3073,25 +3430,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D45" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D46" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D47" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D48" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3222,7 +3579,7 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H17:H18 I17 H22:H23 H27:J27 G1:G1048576 H28">
+  <conditionalFormatting sqref="H17:H18 I17 H22:H23 H27:J27 H28 G1:G1048576">
     <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",G1)))</formula>
     </cfRule>
@@ -3239,7 +3596,7 @@
       <formula>NOT(ISERROR(SEARCH("Finished",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O7">
+  <conditionalFormatting sqref="O3:O8">
     <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",O3)))</formula>
     </cfRule>
@@ -3280,8 +3637,8 @@
   </sheetPr>
   <dimension ref="A1:BO37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -3372,63 +3729,63 @@
     </row>
     <row r="2" spans="1:67" s="7" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
-      <c r="B2" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58"/>
+      <c r="B2" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="61" t="s">
+      <c r="K2" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="63"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="74"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="61" t="s">
+      <c r="Q2" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="63"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="74"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="55" t="s">
+      <c r="V2" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="55" t="s">
+      <c r="AA2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="55"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
       <c r="AH2" s="19"/>
-      <c r="AI2" s="55" t="s">
+      <c r="AI2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
-      <c r="AL2" s="55"/>
-      <c r="AM2" s="55"/>
-      <c r="AN2" s="55"/>
-      <c r="AO2" s="55"/>
-      <c r="AP2" s="55"/>
+      <c r="AJ2" s="63"/>
+      <c r="AK2" s="63"/>
+      <c r="AL2" s="63"/>
+      <c r="AM2" s="63"/>
+      <c r="AN2" s="63"/>
+      <c r="AO2" s="63"/>
+      <c r="AP2" s="63"/>
       <c r="AQ2" s="12"/>
       <c r="AR2" s="12"/>
       <c r="AS2" s="12"/>
@@ -3456,23 +3813,23 @@
       <c r="BO2" s="12"/>
     </row>
     <row r="3" spans="1:67" s="7" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="64" t="s">
-        <v>124</v>
+      <c r="G3" s="69" t="s">
+        <v>118</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>26</v>
@@ -3538,12 +3895,12 @@
       <c r="BO3" s="27"/>
     </row>
     <row r="4" spans="1:67" s="7" customFormat="1" ht="58.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="70"/>
       <c r="H4" s="28">
         <v>44310</v>
       </c>
@@ -3752,12 +4109,12 @@
       <c r="BO4" s="20"/>
     </row>
     <row r="5" spans="1:67" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="71"/>
       <c r="H5" s="21">
         <v>1</v>
       </c>
@@ -4181,7 +4538,7 @@
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B9" s="36" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C9" s="37">
         <v>1</v>
@@ -4261,7 +4618,7 @@
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B10" s="36" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C10" s="37">
         <v>2</v>
@@ -4341,7 +4698,7 @@
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B11" s="36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="37">
         <v>2</v>
@@ -4421,7 +4778,7 @@
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B12" s="36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" s="37">
         <v>3</v>
@@ -4501,7 +4858,7 @@
     </row>
     <row r="13" spans="1:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B13" s="47" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C13" s="48">
         <v>3</v>
@@ -4516,7 +4873,7 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H13" s="49"/>
       <c r="I13" s="49"/>
@@ -4581,7 +4938,7 @@
     </row>
     <row r="14" spans="1:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="48">
         <v>4</v>
@@ -4596,7 +4953,7 @@
         <v>0.25</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
@@ -4661,7 +5018,7 @@
     </row>
     <row r="15" spans="1:67" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="47" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C15" s="48">
         <v>5</v>
@@ -4676,7 +5033,7 @@
         <v>35</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
@@ -4741,22 +5098,22 @@
     </row>
     <row r="16" spans="1:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="47" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
@@ -4821,7 +5178,7 @@
     </row>
     <row r="17" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="51" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C17" s="52">
         <v>4</v>
@@ -4969,7 +5326,7 @@
     </row>
     <row r="19" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="51" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C19" s="52">
         <v>5</v>
@@ -4980,11 +5337,11 @@
       <c r="E19" s="52">
         <v>5</v>
       </c>
-      <c r="F19" s="52" t="s">
-        <v>35</v>
+      <c r="F19" s="52">
+        <v>1</v>
       </c>
       <c r="G19" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
@@ -5049,7 +5406,7 @@
     </row>
     <row r="20" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B20" s="36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" s="37">
         <v>6</v>
@@ -5057,14 +5414,14 @@
       <c r="D20" s="37">
         <v>0.5</v>
       </c>
-      <c r="E20" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>35</v>
+      <c r="E20" s="37">
+        <v>6</v>
+      </c>
+      <c r="F20" s="37">
+        <v>0.5</v>
       </c>
       <c r="G20" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -5129,7 +5486,7 @@
     </row>
     <row r="21" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B21" s="36" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C21" s="37">
         <v>6</v>
@@ -5137,14 +5494,14 @@
       <c r="D21" s="37">
         <v>0.5</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>35</v>
+      <c r="E21" s="37">
+        <v>6</v>
+      </c>
+      <c r="F21" s="37">
+        <v>0.5</v>
       </c>
       <c r="G21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -5207,9 +5564,9 @@
       <c r="BN21" s="12"/>
       <c r="BO21" s="12"/>
     </row>
-    <row r="22" spans="2:67" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:67" ht="34.799999999999997" x14ac:dyDescent="0.35">
       <c r="B22" s="36" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="C22" s="37">
         <v>7</v>
@@ -5217,14 +5574,14 @@
       <c r="D22" s="37">
         <v>0.25</v>
       </c>
-      <c r="E22" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>35</v>
+      <c r="E22" s="37">
+        <v>7</v>
+      </c>
+      <c r="F22" s="37">
+        <v>0.25</v>
       </c>
       <c r="G22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -5289,7 +5646,7 @@
     </row>
     <row r="23" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B23" s="36" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C23" s="37">
         <v>7</v>
@@ -5297,14 +5654,14 @@
       <c r="D23" s="37">
         <v>0.5</v>
       </c>
-      <c r="E23" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="37" t="s">
-        <v>35</v>
+      <c r="E23" s="37">
+        <v>7</v>
+      </c>
+      <c r="F23" s="37">
+        <v>0.25</v>
       </c>
       <c r="G23" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -5369,7 +5726,7 @@
     </row>
     <row r="24" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B24" s="36" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="C24" s="37">
         <v>7</v>
@@ -5377,9 +5734,15 @@
       <c r="D24" s="37">
         <v>0.25</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="23"/>
+      <c r="E24" s="37">
+        <v>8</v>
+      </c>
+      <c r="F24" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="G24" s="23">
+        <v>1</v>
+      </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
@@ -5443,7 +5806,7 @@
     </row>
     <row r="25" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B25" s="36" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="C25" s="37">
         <v>8</v>
@@ -5451,14 +5814,14 @@
       <c r="D25" s="37">
         <v>2</v>
       </c>
-      <c r="E25" s="37" t="s">
-        <v>35</v>
+      <c r="E25" s="37">
+        <v>8</v>
       </c>
       <c r="F25" s="37" t="s">
         <v>35</v>
       </c>
       <c r="G25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
@@ -5523,7 +5886,7 @@
     </row>
     <row r="26" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B26" s="36" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C26" s="37">
         <v>10</v>
@@ -5603,7 +5966,7 @@
     </row>
     <row r="27" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B27" s="36" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C27" s="37">
         <v>10</v>
@@ -5683,7 +6046,7 @@
     </row>
     <row r="28" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B28" s="36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C28" s="37">
         <v>11</v>
@@ -5763,7 +6126,7 @@
     </row>
     <row r="29" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B29" s="36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C29" s="37">
         <v>13</v>
@@ -5843,7 +6206,7 @@
     </row>
     <row r="30" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B30" s="36" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C30" s="37">
         <v>15</v>
@@ -6539,4 +6902,244 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
+  <dimension ref="A2:B97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="75">
+        <v>44331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="75">
+        <v>44332</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="39" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Replace ESP32 Wroom module with WRover and remove the external PSRAM (as Wrover has one built in). Create symbol and footprint for Wrover. Update footprints for resistors and buttons. Update USB footprint as it was not matching symbol.
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3602E4D2-3F79-4E4D-94AA-3202A3920FA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E318E7-D278-41D8-BE99-AF64B38A6453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Outline" sheetId="7" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="201">
   <si>
     <t>Risk</t>
   </si>
@@ -385,9 +385,6 @@
     <t>ESP32 delete video</t>
   </si>
   <si>
-    <t>Develop phone app</t>
-  </si>
-  <si>
     <t>Send video or image via bluetooth on ESP32</t>
   </si>
   <si>
@@ -403,12 +400,6 @@
     <t>Bluetooth ESP32 research</t>
   </si>
   <si>
-    <t>Test buttons</t>
-  </si>
-  <si>
-    <t>Test LEDs</t>
-  </si>
-  <si>
     <t>Bluetooth research on ESP32</t>
   </si>
   <si>
@@ -734,6 +725,18 @@
   </si>
   <si>
     <t>0.3mv Shottky Diodes are relatively expensive (£0.6 each). Will go for 0.39mV as they are £0.23 each and a 1F capacitor to reduce cost (0.47 and 1F capacitor are similar cost)</t>
+  </si>
+  <si>
+    <t>Assign footprints</t>
+  </si>
+  <si>
+    <t>Purchase parts</t>
+  </si>
+  <si>
+    <t>Write firmware</t>
+  </si>
+  <si>
+    <t>Solder parts</t>
   </si>
 </sst>
 </file>
@@ -744,7 +747,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -997,6 +1000,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1227,7 +1238,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1305,8 +1316,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1519,8 +1531,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="29"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="30">
     <cellStyle name="% complete" xfId="17" xr:uid="{8E59E717-42B2-4847-8690-0EA43F601F51}"/>
     <cellStyle name="% complete (beyond plan) legend" xfId="19" xr:uid="{B4647469-F5B5-4FDE-92D9-595F40CB1FB8}"/>
     <cellStyle name="Activity" xfId="3" xr:uid="{39456917-C689-42CC-85A9-756F7255018F}"/>
@@ -1535,6 +1548,7 @@
     <cellStyle name="Heading 3 2" xfId="11" xr:uid="{7520421F-EEA5-4E76-B322-AC9D3615AE9B}"/>
     <cellStyle name="Heading 3 3" xfId="24" xr:uid="{328C38E6-8499-452F-A5A8-1255928A0BE5}"/>
     <cellStyle name="Heading 4 2" xfId="12" xr:uid="{DE7D6760-285C-4405-BCBF-4CA729592816}"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8"/>
     <cellStyle name="Label" xfId="6" xr:uid="{29F17049-0485-42C0-896F-6131C8827C98}"/>
     <cellStyle name="Name" xfId="22" xr:uid="{F8986109-60A4-465A-996E-D8F555625520}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2302,7 +2316,7 @@
     </row>
     <row r="5" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A5" s="44" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -2310,7 +2324,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -2348,12 +2362,12 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="45" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
@@ -2361,7 +2375,7 @@
     </row>
     <row r="20" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2481,7 +2495,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
@@ -2494,7 +2508,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
@@ -2513,8 +2527,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2533,7 +2547,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="60" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="1"/>
@@ -2660,7 +2674,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2689,13 +2703,13 @@
         <v>15</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J8" s="55" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -2818,7 +2832,7 @@
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F15" s="34">
         <v>44310</v>
@@ -2829,7 +2843,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2875,10 +2889,10 @@
         <v>10</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I17" s="57" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2896,7 +2910,7 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F18" s="34">
         <v>44310</v>
@@ -2905,7 +2919,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="57" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2935,12 +2949,12 @@
         <v>44317</v>
       </c>
       <c r="G20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -2956,7 +2970,7 @@
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2983,12 +2997,12 @@
         <v>10</v>
       </c>
       <c r="H22" s="57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -3007,10 +3021,10 @@
         <v>44318</v>
       </c>
       <c r="G23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H23" s="57" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3028,13 +3042,13 @@
         <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F24" s="34">
         <v>44318</v>
       </c>
       <c r="G24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -3045,7 +3059,7 @@
     </row>
     <row r="26" spans="1:10" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -3058,7 +3072,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F26" s="34">
         <v>44324</v>
@@ -3067,18 +3081,18 @@
         <v>10</v>
       </c>
       <c r="H26" s="57" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I26" s="57" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J26" s="57" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -3091,7 +3105,7 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F27" s="34">
         <v>44324</v>
@@ -3100,18 +3114,18 @@
         <v>10</v>
       </c>
       <c r="H27" s="57" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I27" s="57" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J27" s="57" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -3124,7 +3138,7 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F28" s="34">
         <v>44324</v>
@@ -3133,18 +3147,18 @@
         <v>10</v>
       </c>
       <c r="H28" s="57" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I28" s="57" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J28" s="57" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -3192,7 +3206,7 @@
     </row>
     <row r="32" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -3214,13 +3228,13 @@
         <v>10</v>
       </c>
       <c r="H32" s="57" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I32" s="57" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J32" s="57" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -3244,15 +3258,15 @@
         <v>10</v>
       </c>
       <c r="H33" s="57" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I33" s="57" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -3271,15 +3285,15 @@
         <v>10</v>
       </c>
       <c r="H34" s="57" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I34" s="57" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -3292,7 +3306,7 @@
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G35" t="s">
         <v>10</v>
@@ -3300,7 +3314,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -3316,7 +3330,7 @@
         <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -3343,18 +3357,18 @@
         <v>5</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
@@ -3364,33 +3378,33 @@
         <v>5</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="G40" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>199</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
@@ -3411,7 +3425,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -3431,15 +3445,16 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>92</v>
-      </c>
+      <c r="A44" s="39"/>
       <c r="B44" t="s">
         <v>3</v>
       </c>
@@ -3458,120 +3473,135 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>98</v>
+      </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D49" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>89</v>
+      </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D51" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D52" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D53" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D54" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D55" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D56" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D57" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D58" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D59" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D61" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D62" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D64" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3662,10 +3692,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO37"/>
+  <dimension ref="A1:BO38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -3757,7 +3787,7 @@
     <row r="2" spans="1:67" s="7" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
       <c r="B2" s="65" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
@@ -3767,7 +3797,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="15"/>
@@ -3856,7 +3886,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>26</v>
@@ -4565,7 +4595,7 @@
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B9" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C9" s="37">
         <v>1</v>
@@ -4645,7 +4675,7 @@
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B10" s="36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C10" s="37">
         <v>2</v>
@@ -4885,7 +4915,7 @@
     </row>
     <row r="13" spans="1:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B13" s="47" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C13" s="48">
         <v>3</v>
@@ -4900,7 +4930,7 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H13" s="49"/>
       <c r="I13" s="49"/>
@@ -4980,7 +5010,7 @@
         <v>0.25</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
@@ -5045,7 +5075,7 @@
     </row>
     <row r="15" spans="1:67" s="46" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="48">
         <v>5</v>
@@ -5060,7 +5090,7 @@
         <v>35</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
@@ -5125,22 +5155,22 @@
     </row>
     <row r="16" spans="1:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
@@ -5205,7 +5235,7 @@
     </row>
     <row r="17" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="51" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C17" s="52">
         <v>4</v>
@@ -5353,7 +5383,7 @@
     </row>
     <row r="19" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="51" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C19" s="52">
         <v>5</v>
@@ -5433,7 +5463,7 @@
     </row>
     <row r="20" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B20" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="37">
         <v>6</v>
@@ -5513,7 +5543,7 @@
     </row>
     <row r="21" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B21" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="37">
         <v>6</v>
@@ -5593,7 +5623,7 @@
     </row>
     <row r="22" spans="2:67" ht="34.799999999999997" x14ac:dyDescent="0.35">
       <c r="B22" s="36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C22" s="37">
         <v>7</v>
@@ -5673,7 +5703,7 @@
     </row>
     <row r="23" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B23" s="36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C23" s="37">
         <v>7</v>
@@ -5753,7 +5783,7 @@
     </row>
     <row r="24" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B24" s="36" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C24" s="37">
         <v>7</v>
@@ -5833,7 +5863,7 @@
     </row>
     <row r="25" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B25" s="36" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C25" s="37">
         <v>8</v>
@@ -5844,11 +5874,11 @@
       <c r="E25" s="37">
         <v>8</v>
       </c>
-      <c r="F25" s="37" t="s">
-        <v>35</v>
+      <c r="F25" s="37">
+        <v>1.5</v>
       </c>
       <c r="G25" s="23">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
@@ -5913,7 +5943,7 @@
     </row>
     <row r="26" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B26" s="36" t="s">
-        <v>89</v>
+        <v>197</v>
       </c>
       <c r="C26" s="37">
         <v>10</v>
@@ -5921,14 +5951,14 @@
       <c r="D26" s="37">
         <v>0.5</v>
       </c>
-      <c r="E26" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>35</v>
+      <c r="E26" s="37">
+        <v>9</v>
+      </c>
+      <c r="F26" s="37">
+        <v>0.5</v>
       </c>
       <c r="G26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
@@ -5993,16 +6023,16 @@
     </row>
     <row r="27" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B27" s="36" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C27" s="37">
         <v>10</v>
       </c>
       <c r="D27" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>35</v>
+        <v>3</v>
+      </c>
+      <c r="E27" s="37">
+        <v>10</v>
       </c>
       <c r="F27" s="37" t="s">
         <v>35</v>
@@ -6073,16 +6103,16 @@
     </row>
     <row r="28" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B28" s="36" t="s">
-        <v>79</v>
+        <v>198</v>
       </c>
       <c r="C28" s="37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" s="37">
-        <v>2</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>35</v>
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="37">
+        <v>10</v>
       </c>
       <c r="F28" s="37" t="s">
         <v>35</v>
@@ -6153,13 +6183,13 @@
     </row>
     <row r="29" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B29" s="36" t="s">
-        <v>83</v>
+        <v>199</v>
       </c>
       <c r="C29" s="37">
         <v>13</v>
       </c>
       <c r="D29" s="37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>35</v>
@@ -6233,23 +6263,17 @@
     </row>
     <row r="30" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B30" s="36" t="s">
-        <v>92</v>
+        <v>200</v>
       </c>
       <c r="C30" s="37">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D30" s="37">
-        <v>4</v>
-      </c>
-      <c r="E30" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="G30" s="23">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
@@ -6313,13 +6337,13 @@
     </row>
     <row r="31" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B31" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>35</v>
+        <v>89</v>
+      </c>
+      <c r="C31" s="37">
+        <v>13</v>
+      </c>
+      <c r="D31" s="37">
+        <v>2</v>
       </c>
       <c r="E31" s="37" t="s">
         <v>35</v>
@@ -6871,6 +6895,86 @@
       <c r="BN37" s="12"/>
       <c r="BO37" s="12"/>
     </row>
+    <row r="38" spans="2:67" x14ac:dyDescent="0.35">
+      <c r="B38" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" s="23">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="12"/>
+      <c r="AC38" s="12"/>
+      <c r="AD38" s="12"/>
+      <c r="AE38" s="12"/>
+      <c r="AF38" s="12"/>
+      <c r="AG38" s="12"/>
+      <c r="AH38" s="12"/>
+      <c r="AI38" s="12"/>
+      <c r="AJ38" s="12"/>
+      <c r="AK38" s="12"/>
+      <c r="AL38" s="12"/>
+      <c r="AM38" s="12"/>
+      <c r="AN38" s="12"/>
+      <c r="AO38" s="12"/>
+      <c r="AP38" s="12"/>
+      <c r="AQ38" s="12"/>
+      <c r="AR38" s="12"/>
+      <c r="AS38" s="12"/>
+      <c r="AT38" s="12"/>
+      <c r="AU38" s="12"/>
+      <c r="AV38" s="12"/>
+      <c r="AW38" s="12"/>
+      <c r="AX38" s="12"/>
+      <c r="AY38" s="12"/>
+      <c r="AZ38" s="12"/>
+      <c r="BA38" s="12"/>
+      <c r="BB38" s="12"/>
+      <c r="BC38" s="12"/>
+      <c r="BD38" s="12"/>
+      <c r="BE38" s="12"/>
+      <c r="BF38" s="12"/>
+      <c r="BG38" s="12"/>
+      <c r="BH38" s="12"/>
+      <c r="BI38" s="12"/>
+      <c r="BJ38" s="12"/>
+      <c r="BK38" s="12"/>
+      <c r="BL38" s="12"/>
+      <c r="BM38" s="12"/>
+      <c r="BN38" s="12"/>
+      <c r="BO38" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="V2:Y2"/>
@@ -6886,7 +6990,7 @@
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H6:BO37">
+  <conditionalFormatting sqref="H6:BO38">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -6912,7 +7016,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38:BO38">
+  <conditionalFormatting sqref="B39:BO39">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -6935,8 +7039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
   <dimension ref="A2:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6951,57 +7055,57 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -7011,87 +7115,87 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="39" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
@@ -7104,10 +7208,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>15</v>
@@ -7115,140 +7219,149 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C82" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C83" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D83" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D84" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C85" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C86" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C87" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C88" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D88" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C90" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C91" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C93" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94" t="s">
         <v>192</v>
       </c>
-      <c r="D94" t="s">
-        <v>195</v>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="59">
+        <v>44339</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>186</v>
+      <c r="A102" s="76" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>187</v>
+      <c r="A103" s="76" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A102" r:id="rId1" xr:uid="{0C0E7329-B2B4-4E4B-9855-FE0B5531AD24}"/>
+    <hyperlink ref="A103" r:id="rId2" xr:uid="{F6B97EAE-B2BF-4AFA-A709-A0C800DF4B1C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add correct 3d model for esp32 wrover e. initial placement of components done for both boards. need to start routing
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F455E082-1D02-4146-9BC3-38E9A6DED3C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98B6073-9F9F-4FF6-92E0-C1E4A849DD20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="224">
   <si>
     <t>Risk</t>
   </si>
@@ -782,6 +782,30 @@
   </si>
   <si>
     <t>If space, add SD card here so the only thing on the other PCB is the lower priority I2C peripherals only.</t>
+  </si>
+  <si>
+    <t>Working on PCB design and continuing working out which components go to which PCB.</t>
+  </si>
+  <si>
+    <t>New design:</t>
+  </si>
+  <si>
+    <t>SD card</t>
+  </si>
+  <si>
+    <t>Power LED</t>
+  </si>
+  <si>
+    <t>Researched prices of 2 vs 4 layer pcbs. JLC PCB seems to be a lot cheaper than the alernatives (i.e. PCBWAY). There is only a small difference between 2 and 4 layer board. Will design 4 layer board.</t>
+  </si>
+  <si>
+    <t>Decided against having the SD card on a separate board due to worries that the SPI comms may corrupt.</t>
+  </si>
+  <si>
+    <t>Made progress on PCB design.</t>
+  </si>
+  <si>
+    <t>Made further progress on PCB design. Components placed,  need to route tracks.</t>
   </si>
 </sst>
 </file>
@@ -1893,9 +1917,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>436667</xdr:colOff>
+      <xdr:colOff>440477</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>130618</xdr:rowOff>
+      <xdr:rowOff>134428</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1939,7 +1963,7 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>267880</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>169046</xdr:rowOff>
+      <xdr:rowOff>172856</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1981,7 +2005,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>580190</xdr:colOff>
+      <xdr:colOff>587810</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>115642</xdr:rowOff>
     </xdr:to>
@@ -2025,9 +2049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>176980</xdr:rowOff>
+      <xdr:rowOff>173170</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7054,10 +7078,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
-  <dimension ref="A2:D158"/>
+  <dimension ref="A2:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7465,6 +7489,107 @@
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>209</v>
+      </c>
+      <c r="D158" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D159" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="59">
+        <v>44353</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>205</v>
+      </c>
+      <c r="D170" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>206</v>
+      </c>
+      <c r="D171" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>214</v>
+      </c>
+      <c r="D172" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>208</v>
+      </c>
+      <c r="D173" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>209</v>
+      </c>
+      <c r="D174" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D175" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" s="59">
+        <v>44359</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'productionize' the hardware. update project plan spreadsheet'
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98B6073-9F9F-4FF6-92E0-C1E4A849DD20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE314A6-FBC8-41B3-8A4E-B36E472C83A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="231">
   <si>
     <t>Risk</t>
   </si>
@@ -806,6 +806,27 @@
   </si>
   <si>
     <t>Made further progress on PCB design. Components placed,  need to route tracks.</t>
+  </si>
+  <si>
+    <t>Finished routing tracks for front PCB</t>
+  </si>
+  <si>
+    <t>Finished routing tracks for back PCB. Ran DRC check and passing. All tracks routes (except the 5 that are going to be connected via A FPC).</t>
+  </si>
+  <si>
+    <t>Connected the two boards together with mouse bites.</t>
+  </si>
+  <si>
+    <t>JLCPCB charges ~£30 extra for vias smaller than 0.45 mm…</t>
+  </si>
+  <si>
+    <t>JLCPCB also charges an extra £30 for multi-panel designs.</t>
+  </si>
+  <si>
+    <t>I sent it off anyway as both 'panels' are the same width/height, hopefully they accept review.</t>
+  </si>
+  <si>
+    <t>If they accept review, I may buy their SMT service.</t>
   </si>
 </sst>
 </file>
@@ -1917,9 +1938,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>440477</xdr:colOff>
+      <xdr:colOff>436667</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>134428</xdr:rowOff>
+      <xdr:rowOff>130618</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1963,7 +1984,7 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>267880</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>172856</xdr:rowOff>
+      <xdr:rowOff>169046</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2005,7 +2026,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>587810</xdr:colOff>
+      <xdr:colOff>591620</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>115642</xdr:rowOff>
     </xdr:to>
@@ -2049,9 +2070,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>173170</xdr:rowOff>
+      <xdr:rowOff>169360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7078,10 +7099,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
-  <dimension ref="A2:D184"/>
+  <dimension ref="A2:D199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A185" sqref="A185"/>
+      <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7590,6 +7611,51 @@
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" s="59">
+        <v>44396</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" s="59">
+        <v>44397</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to latest gerbers, update project plan
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE314A6-FBC8-41B3-8A4E-B36E472C83A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E321C7AB-5294-47AA-9BCA-B7019A21B38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Outline" sheetId="7" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="255">
   <si>
     <t>Risk</t>
   </si>
@@ -445,9 +445,6 @@
     <t>Notes 2</t>
   </si>
   <si>
-    <t>Using jamezah's esp32 code to save jpegs to AVI files. Confirmed it works.</t>
-  </si>
-  <si>
     <t>It's possible to make an app using Flutter. However decided to put this on hold because it has a steep learning curve relative to the rest of the project and high risk in terms of getting it to work as I've not had experience building phone apps.</t>
   </si>
   <si>
@@ -736,9 +733,6 @@
     <t xml:space="preserve">After analyzing the mechanical specification- I noticed the OLED has 0.62mm pitch (not 0.5 mm like previously assumed). </t>
   </si>
   <si>
-    <t>The plan is now to have 2 PCBs (which essentially doubles the surface area for components) and make it thicker. The idea is that this will distribute the lengths evenly across all 3 axis thus making the device appear smaller to the driver.</t>
-  </si>
-  <si>
     <t>PERIODS</t>
   </si>
   <si>
@@ -811,9 +805,6 @@
     <t>Finished routing tracks for front PCB</t>
   </si>
   <si>
-    <t>Finished routing tracks for back PCB. Ran DRC check and passing. All tracks routes (except the 5 that are going to be connected via A FPC).</t>
-  </si>
-  <si>
     <t>Connected the two boards together with mouse bites.</t>
   </si>
   <si>
@@ -827,6 +818,87 @@
   </si>
   <si>
     <t>If they accept review, I may buy their SMT service.</t>
+  </si>
+  <si>
+    <t>Finished routing tracks for back PCB. Ran DRC check and passing. All tracks routes (except the 5 that are going to be connected via A FPC as expected).</t>
+  </si>
+  <si>
+    <t>JLCPCB accepted the review.</t>
+  </si>
+  <si>
+    <t>Choosing parts from JLCPCB, updating schem to include their part numbers. Will order the rest from Digikey</t>
+  </si>
+  <si>
+    <t>JLCPCB charged extra because my PCB has "two designs".</t>
+  </si>
+  <si>
+    <t>The PCBs arrived this week. There is some soldering left to do. My aim is to solder the rest of the components, then test each section.</t>
+  </si>
+  <si>
+    <t>Test PCB</t>
+  </si>
+  <si>
+    <t>Order and wait for PCB</t>
+  </si>
+  <si>
+    <t>Some changes need to be made to the PCB:</t>
+  </si>
+  <si>
+    <t>1. Use a different FFC connector for the connection of the two boards. There is only a few wires needed anyway, using 24 way 0.5 mm pitch is too hard to solder without giving any benefits.</t>
+  </si>
+  <si>
+    <t>2. Leave more space  between the mounting holes as components get in the way of the hex nuts</t>
+  </si>
+  <si>
+    <t>3. The SD card connector was back to front. The side where you solder IS the side where the SD card connects to…</t>
+  </si>
+  <si>
+    <t>4. Update footprint of the buttons, currently they have 3 GNDs but the actual buttons themselves only has 2 grounds in opposite corners.</t>
+  </si>
+  <si>
+    <t>5. Increase via size to minimum from JLCPcb so the PCBs are cheaper?</t>
+  </si>
+  <si>
+    <t>Going to see if the ESP32 works with the current connections.</t>
+  </si>
+  <si>
+    <t>Using jamezah's esp32 code to save jpegs to AVI files. Tested and confirm it works (records video and saves to sd card)</t>
+  </si>
+  <si>
+    <t>Did some initial research and it seems this will add too much complexity to the firmware. Will use alternative for first product which is a HTTP server that can be accessed via internet hotspot.</t>
+  </si>
+  <si>
+    <t>Soldering mostly complete however the board must be redesigned.</t>
+  </si>
+  <si>
+    <t>6. Add silkscreen for the esp32 uart connector.</t>
+  </si>
+  <si>
+    <t>PCB Spin 2</t>
+  </si>
+  <si>
+    <t>Solder PCB 2</t>
+  </si>
+  <si>
+    <t>Confirm the ESP32 can be programmed and can receive/transmit via UART</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Buy more OLEDs, as they take a while to deliver</t>
+  </si>
+  <si>
+    <t>Check other components that we may need now that some of them were using during soldering</t>
+  </si>
+  <si>
+    <t>Buy twice as many as components needed, accidents happen more often than I thought they would</t>
+  </si>
+  <si>
+    <t>First day of soldering: Using Hakko soldering iron with unleaded solder and flux, the soldering was relatively straight forward after I started using flux. Everything has been soldered on except the 24 way connectors.</t>
+  </si>
+  <si>
+    <t>The 24 way FFC connectors proved very difficult. I believe I must use a hot air gun, because the pins short very easily with a soldering iron and it's difficult to remove the shorts.</t>
   </si>
 </sst>
 </file>
@@ -1938,9 +2010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>436667</xdr:colOff>
+      <xdr:colOff>440477</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>130618</xdr:rowOff>
+      <xdr:rowOff>134428</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1984,7 +2056,7 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>267880</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>169046</xdr:rowOff>
+      <xdr:rowOff>172856</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2026,7 +2098,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>591620</xdr:colOff>
+      <xdr:colOff>587810</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>115642</xdr:rowOff>
     </xdr:to>
@@ -2070,9 +2142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>169360</xdr:rowOff>
+      <xdr:rowOff>173170</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2426,7 +2498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F592D8-4C2B-4170-A862-E2D8CBA58E18}">
   <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
@@ -2626,7 +2698,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
@@ -2639,7 +2711,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
@@ -2659,7 +2731,7 @@
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2820,10 +2892,10 @@
         <v>102</v>
       </c>
       <c r="I8" s="55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -2961,7 +3033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2985,7 +3057,7 @@
         <v>96</v>
       </c>
       <c r="H17" s="57" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -3018,7 +3090,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -3036,7 +3108,10 @@
         <v>44317</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -3054,7 +3129,7 @@
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -3099,10 +3174,10 @@
         <v>44318</v>
       </c>
       <c r="F23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G23" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -3123,7 +3198,7 @@
         <v>44318</v>
       </c>
       <c r="F24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -3134,7 +3209,7 @@
     </row>
     <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -3153,18 +3228,18 @@
         <v>6</v>
       </c>
       <c r="G26" s="57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H26" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="I26" s="57" t="s">
         <v>147</v>
-      </c>
-      <c r="I26" s="57" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -3183,18 +3258,18 @@
         <v>6</v>
       </c>
       <c r="G27" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="H27" s="57" t="s">
+      <c r="I27" s="57" t="s">
         <v>116</v>
-      </c>
-      <c r="I27" s="57" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -3213,18 +3288,18 @@
         <v>6</v>
       </c>
       <c r="G28" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H28" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="57" t="s">
         <v>119</v>
-      </c>
-      <c r="I28" s="57" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -3285,13 +3360,13 @@
         <v>6</v>
       </c>
       <c r="G32" s="57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H32" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="I32" s="57" t="s">
         <v>149</v>
-      </c>
-      <c r="I32" s="57" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -3312,15 +3387,15 @@
         <v>6</v>
       </c>
       <c r="G33" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" s="57" t="s">
         <v>151</v>
-      </c>
-      <c r="H33" s="57" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -3336,15 +3411,15 @@
         <v>6</v>
       </c>
       <c r="G34" s="57" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H34" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -3362,7 +3437,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -3404,7 +3479,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
@@ -3422,7 +3497,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -3435,12 +3510,12 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -3453,12 +3528,12 @@
         <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
@@ -3471,7 +3546,7 @@
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -3483,9 +3558,9 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
@@ -3498,17 +3573,16 @@
         <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="G45" s="57" t="s">
-        <v>197</v>
-      </c>
-      <c r="H45" s="57" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="39"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="39" t="s">
+        <v>192</v>
+      </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
@@ -3520,7 +3594,10 @@
         <v>55</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="G46" s="57" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -3754,10 +3831,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO38"/>
+  <dimension ref="A1:BO41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -3859,7 +3936,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="14">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="15"/>
@@ -3948,10 +4025,10 @@
         <v>21</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="26"/>
@@ -4992,7 +5069,7 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H13" s="49"/>
       <c r="I13" s="49"/>
@@ -5072,7 +5149,7 @@
         <v>0.25</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
@@ -5152,7 +5229,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
@@ -5220,19 +5297,19 @@
         <v>94</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
@@ -5297,7 +5374,7 @@
     </row>
     <row r="17" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="52">
         <v>4</v>
@@ -5376,12 +5453,24 @@
       <c r="BO17" s="50"/>
     </row>
     <row r="18" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="23"/>
+      <c r="B18" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="52">
+        <v>5</v>
+      </c>
+      <c r="D18" s="52">
+        <v>1</v>
+      </c>
+      <c r="E18" s="52">
+        <v>5</v>
+      </c>
+      <c r="F18" s="52">
+        <v>1</v>
+      </c>
+      <c r="G18" s="23">
+        <v>1</v>
+      </c>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
@@ -5443,89 +5532,89 @@
       <c r="BN18" s="50"/>
       <c r="BO18" s="50"/>
     </row>
-    <row r="19" spans="2:67" s="46" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="52">
-        <v>5</v>
-      </c>
-      <c r="D19" s="52">
-        <v>1</v>
-      </c>
-      <c r="E19" s="52">
-        <v>5</v>
-      </c>
-      <c r="F19" s="52">
-        <v>1</v>
+    <row r="19" spans="2:67" x14ac:dyDescent="0.35">
+      <c r="B19" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="37">
+        <v>6</v>
+      </c>
+      <c r="D19" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="37">
+        <v>6</v>
+      </c>
+      <c r="F19" s="37">
+        <v>0.5</v>
       </c>
       <c r="G19" s="23">
         <v>1</v>
       </c>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="49"/>
-      <c r="U19" s="49"/>
-      <c r="V19" s="49"/>
-      <c r="W19" s="49"/>
-      <c r="X19" s="49"/>
-      <c r="Y19" s="49"/>
-      <c r="Z19" s="49"/>
-      <c r="AA19" s="49"/>
-      <c r="AB19" s="50"/>
-      <c r="AC19" s="50"/>
-      <c r="AD19" s="50"/>
-      <c r="AE19" s="50"/>
-      <c r="AF19" s="50"/>
-      <c r="AG19" s="50"/>
-      <c r="AH19" s="50"/>
-      <c r="AI19" s="50"/>
-      <c r="AJ19" s="50"/>
-      <c r="AK19" s="50"/>
-      <c r="AL19" s="50"/>
-      <c r="AM19" s="50"/>
-      <c r="AN19" s="50"/>
-      <c r="AO19" s="50"/>
-      <c r="AP19" s="50"/>
-      <c r="AQ19" s="50"/>
-      <c r="AR19" s="50"/>
-      <c r="AS19" s="50"/>
-      <c r="AT19" s="50"/>
-      <c r="AU19" s="50"/>
-      <c r="AV19" s="50"/>
-      <c r="AW19" s="50"/>
-      <c r="AX19" s="50"/>
-      <c r="AY19" s="50"/>
-      <c r="AZ19" s="50"/>
-      <c r="BA19" s="50"/>
-      <c r="BB19" s="50"/>
-      <c r="BC19" s="50"/>
-      <c r="BD19" s="50"/>
-      <c r="BE19" s="50"/>
-      <c r="BF19" s="50"/>
-      <c r="BG19" s="50"/>
-      <c r="BH19" s="50"/>
-      <c r="BI19" s="50"/>
-      <c r="BJ19" s="50"/>
-      <c r="BK19" s="50"/>
-      <c r="BL19" s="50"/>
-      <c r="BM19" s="50"/>
-      <c r="BN19" s="50"/>
-      <c r="BO19" s="50"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="12"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+      <c r="AM19" s="12"/>
+      <c r="AN19" s="12"/>
+      <c r="AO19" s="12"/>
+      <c r="AP19" s="12"/>
+      <c r="AQ19" s="12"/>
+      <c r="AR19" s="12"/>
+      <c r="AS19" s="12"/>
+      <c r="AT19" s="12"/>
+      <c r="AU19" s="12"/>
+      <c r="AV19" s="12"/>
+      <c r="AW19" s="12"/>
+      <c r="AX19" s="12"/>
+      <c r="AY19" s="12"/>
+      <c r="AZ19" s="12"/>
+      <c r="BA19" s="12"/>
+      <c r="BB19" s="12"/>
+      <c r="BC19" s="12"/>
+      <c r="BD19" s="12"/>
+      <c r="BE19" s="12"/>
+      <c r="BF19" s="12"/>
+      <c r="BG19" s="12"/>
+      <c r="BH19" s="12"/>
+      <c r="BI19" s="12"/>
+      <c r="BJ19" s="12"/>
+      <c r="BK19" s="12"/>
+      <c r="BL19" s="12"/>
+      <c r="BM19" s="12"/>
+      <c r="BN19" s="12"/>
+      <c r="BO19" s="12"/>
     </row>
     <row r="20" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B20" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="37">
         <v>6</v>
@@ -5603,21 +5692,21 @@
       <c r="BN20" s="12"/>
       <c r="BO20" s="12"/>
     </row>
-    <row r="21" spans="2:67" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:67" ht="34.799999999999997" x14ac:dyDescent="0.35">
       <c r="B21" s="36" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="C21" s="37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21" s="37">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E21" s="37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F21" s="37">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G21" s="23">
         <v>1</v>
@@ -5683,7 +5772,7 @@
       <c r="BN21" s="12"/>
       <c r="BO21" s="12"/>
     </row>
-    <row r="22" spans="2:67" ht="34.799999999999997" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B22" s="36" t="s">
         <v>124</v>
       </c>
@@ -5691,7 +5780,7 @@
         <v>7</v>
       </c>
       <c r="D22" s="37">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="37">
         <v>7</v>
@@ -5765,16 +5854,16 @@
     </row>
     <row r="23" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B23" s="36" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C23" s="37">
         <v>7</v>
       </c>
       <c r="D23" s="37">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F23" s="37">
         <v>0.25</v>
@@ -5845,19 +5934,19 @@
     </row>
     <row r="24" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B24" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="37">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="37">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="E24" s="37">
         <v>8</v>
       </c>
       <c r="F24" s="37">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="G24" s="23">
         <v>1</v>
@@ -5925,19 +6014,19 @@
     </row>
     <row r="25" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B25" s="36" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="C25" s="37">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25" s="37">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="37">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F25" s="37">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="23">
         <v>1</v>
@@ -6005,19 +6094,19 @@
     </row>
     <row r="26" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B26" s="36" t="s">
-        <v>190</v>
+        <v>74</v>
       </c>
       <c r="C26" s="37">
         <v>10</v>
       </c>
       <c r="D26" s="37">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="37">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F26" s="37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26" s="23">
         <v>1</v>
@@ -6085,22 +6174,22 @@
     </row>
     <row r="27" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B27" s="36" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="C27" s="37">
         <v>10</v>
       </c>
       <c r="D27" s="37">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E27" s="37">
-        <v>12</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="F27" s="37">
+        <v>1</v>
       </c>
       <c r="G27" s="23">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
@@ -6165,22 +6254,22 @@
     </row>
     <row r="28" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B28" s="36" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="C28" s="37">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D28" s="37">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="37">
-        <v>10</v>
-      </c>
-      <c r="F28" s="37" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="F28" s="37">
+        <v>12</v>
       </c>
       <c r="G28" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
@@ -6248,19 +6337,19 @@
         <v>192</v>
       </c>
       <c r="C29" s="37">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D29" s="37">
-        <v>5</v>
-      </c>
-      <c r="E29" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="37" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="E29" s="37">
+        <v>26</v>
+      </c>
+      <c r="F29" s="37">
+        <v>2</v>
       </c>
       <c r="G29" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -6325,13 +6414,13 @@
     </row>
     <row r="30" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B30" s="36" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="C30" s="37">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D30" s="37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="37"/>
       <c r="F30" s="37"/>
@@ -6399,23 +6488,13 @@
     </row>
     <row r="31" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B31" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="37">
-        <v>13</v>
-      </c>
-      <c r="D31" s="37">
-        <v>2</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="23">
-        <v>0</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
@@ -6479,20 +6558,16 @@
     </row>
     <row r="32" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B32" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="37" t="s">
-        <v>30</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="C32" s="37">
+        <v>18</v>
+      </c>
+      <c r="D32" s="37">
+        <v>2</v>
+      </c>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="23">
         <v>0</v>
       </c>
@@ -6559,13 +6634,13 @@
     </row>
     <row r="33" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B33" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>30</v>
+        <v>191</v>
+      </c>
+      <c r="C33" s="37">
+        <v>20</v>
+      </c>
+      <c r="D33" s="37">
+        <v>5</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>30</v>
@@ -6639,13 +6714,13 @@
     </row>
     <row r="34" spans="2:67" x14ac:dyDescent="0.35">
       <c r="B34" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>30</v>
+        <v>84</v>
+      </c>
+      <c r="C34" s="37">
+        <v>26</v>
+      </c>
+      <c r="D34" s="37">
+        <v>2</v>
       </c>
       <c r="E34" s="37" t="s">
         <v>30</v>
@@ -7037,6 +7112,246 @@
       <c r="BN38" s="12"/>
       <c r="BO38" s="12"/>
     </row>
+    <row r="39" spans="2:67" x14ac:dyDescent="0.35">
+      <c r="B39" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" s="23">
+        <v>0</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="12"/>
+      <c r="AC39" s="12"/>
+      <c r="AD39" s="12"/>
+      <c r="AE39" s="12"/>
+      <c r="AF39" s="12"/>
+      <c r="AG39" s="12"/>
+      <c r="AH39" s="12"/>
+      <c r="AI39" s="12"/>
+      <c r="AJ39" s="12"/>
+      <c r="AK39" s="12"/>
+      <c r="AL39" s="12"/>
+      <c r="AM39" s="12"/>
+      <c r="AN39" s="12"/>
+      <c r="AO39" s="12"/>
+      <c r="AP39" s="12"/>
+      <c r="AQ39" s="12"/>
+      <c r="AR39" s="12"/>
+      <c r="AS39" s="12"/>
+      <c r="AT39" s="12"/>
+      <c r="AU39" s="12"/>
+      <c r="AV39" s="12"/>
+      <c r="AW39" s="12"/>
+      <c r="AX39" s="12"/>
+      <c r="AY39" s="12"/>
+      <c r="AZ39" s="12"/>
+      <c r="BA39" s="12"/>
+      <c r="BB39" s="12"/>
+      <c r="BC39" s="12"/>
+      <c r="BD39" s="12"/>
+      <c r="BE39" s="12"/>
+      <c r="BF39" s="12"/>
+      <c r="BG39" s="12"/>
+      <c r="BH39" s="12"/>
+      <c r="BI39" s="12"/>
+      <c r="BJ39" s="12"/>
+      <c r="BK39" s="12"/>
+      <c r="BL39" s="12"/>
+      <c r="BM39" s="12"/>
+      <c r="BN39" s="12"/>
+      <c r="BO39" s="12"/>
+    </row>
+    <row r="40" spans="2:67" x14ac:dyDescent="0.35">
+      <c r="B40" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="23">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="12"/>
+      <c r="AC40" s="12"/>
+      <c r="AD40" s="12"/>
+      <c r="AE40" s="12"/>
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+      <c r="AH40" s="12"/>
+      <c r="AI40" s="12"/>
+      <c r="AJ40" s="12"/>
+      <c r="AK40" s="12"/>
+      <c r="AL40" s="12"/>
+      <c r="AM40" s="12"/>
+      <c r="AN40" s="12"/>
+      <c r="AO40" s="12"/>
+      <c r="AP40" s="12"/>
+      <c r="AQ40" s="12"/>
+      <c r="AR40" s="12"/>
+      <c r="AS40" s="12"/>
+      <c r="AT40" s="12"/>
+      <c r="AU40" s="12"/>
+      <c r="AV40" s="12"/>
+      <c r="AW40" s="12"/>
+      <c r="AX40" s="12"/>
+      <c r="AY40" s="12"/>
+      <c r="AZ40" s="12"/>
+      <c r="BA40" s="12"/>
+      <c r="BB40" s="12"/>
+      <c r="BC40" s="12"/>
+      <c r="BD40" s="12"/>
+      <c r="BE40" s="12"/>
+      <c r="BF40" s="12"/>
+      <c r="BG40" s="12"/>
+      <c r="BH40" s="12"/>
+      <c r="BI40" s="12"/>
+      <c r="BJ40" s="12"/>
+      <c r="BK40" s="12"/>
+      <c r="BL40" s="12"/>
+      <c r="BM40" s="12"/>
+      <c r="BN40" s="12"/>
+      <c r="BO40" s="12"/>
+    </row>
+    <row r="41" spans="2:67" x14ac:dyDescent="0.35">
+      <c r="B41" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="23">
+        <v>0</v>
+      </c>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="12"/>
+      <c r="AD41" s="12"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="12"/>
+      <c r="AH41" s="12"/>
+      <c r="AI41" s="12"/>
+      <c r="AJ41" s="12"/>
+      <c r="AK41" s="12"/>
+      <c r="AL41" s="12"/>
+      <c r="AM41" s="12"/>
+      <c r="AN41" s="12"/>
+      <c r="AO41" s="12"/>
+      <c r="AP41" s="12"/>
+      <c r="AQ41" s="12"/>
+      <c r="AR41" s="12"/>
+      <c r="AS41" s="12"/>
+      <c r="AT41" s="12"/>
+      <c r="AU41" s="12"/>
+      <c r="AV41" s="12"/>
+      <c r="AW41" s="12"/>
+      <c r="AX41" s="12"/>
+      <c r="AY41" s="12"/>
+      <c r="AZ41" s="12"/>
+      <c r="BA41" s="12"/>
+      <c r="BB41" s="12"/>
+      <c r="BC41" s="12"/>
+      <c r="BD41" s="12"/>
+      <c r="BE41" s="12"/>
+      <c r="BF41" s="12"/>
+      <c r="BG41" s="12"/>
+      <c r="BH41" s="12"/>
+      <c r="BI41" s="12"/>
+      <c r="BJ41" s="12"/>
+      <c r="BK41" s="12"/>
+      <c r="BL41" s="12"/>
+      <c r="BM41" s="12"/>
+      <c r="BN41" s="12"/>
+      <c r="BO41" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="V2:Y2"/>
@@ -7052,7 +7367,7 @@
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H6:BO38">
+  <conditionalFormatting sqref="H6:BO41">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -7078,7 +7393,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:BO39">
+  <conditionalFormatting sqref="B42:BO42">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
@@ -7099,10 +7414,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
-  <dimension ref="A2:D199"/>
+  <dimension ref="A2:D239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201"/>
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A218" sqref="A218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7117,57 +7432,57 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
@@ -7177,87 +7492,87 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
@@ -7270,10 +7585,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>11</v>
@@ -7281,115 +7596,115 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D84" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" t="s">
+        <v>106</v>
+      </c>
+      <c r="D88" t="s">
         <v>187</v>
-      </c>
-      <c r="C88" t="s">
-        <v>107</v>
-      </c>
-      <c r="D88" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C92" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C93" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
@@ -7399,22 +7714,22 @@
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
@@ -7424,12 +7739,12 @@
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
@@ -7439,17 +7754,17 @@
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -7459,65 +7774,65 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D154" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D155" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D156" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D157" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D158" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D159" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -7527,80 +7842,80 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D170" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D171" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D172" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D173" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D174" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D175" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
@@ -7610,52 +7925,164 @@
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="59">
-        <v>44396</v>
+        <v>44366</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="59">
-        <v>44397</v>
+        <v>44367</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" s="59">
+        <v>44374</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" s="59">
+        <v>44395</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" s="59">
+        <v>44402</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new update to project log. all 3 24-way fpc's connected. will continue validating hardware and make relevant changes for spin 2
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E321C7AB-5294-47AA-9BCA-B7019A21B38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71648E89-6A48-4144-ACE2-8142B8E37676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="263">
   <si>
     <t>Risk</t>
   </si>
@@ -899,6 +899,53 @@
   </si>
   <si>
     <t>The 24 way FFC connectors proved very difficult. I believe I must use a hot air gun, because the pins short very easily with a soldering iron and it's difficult to remove the shorts.</t>
+  </si>
+  <si>
+    <t>Purchased a hot air gun and solder paste to solder the 0.5 mm pitch 24-way FPC connectors, and it was very successful.</t>
+  </si>
+  <si>
+    <t>Hot air gun at 450 degrees with 20% air flow. Add solder paste across the connectors in a thin line. Scrape off excess/flatten with toothpick. Then apply hot air for around 30 seconds whilst going round in circles.</t>
+  </si>
+  <si>
+    <t>Sometimes the pins will bridge, if they do then use a de-soldering braid to de-solder- removes very easily.</t>
+  </si>
+  <si>
+    <t>Other times the connection to the pin isn't made. So test with multimeter to ensure connectivity. If not connected, add a tiny bit of solder paste around that pin and pad, then touch the tip of a hot soldering iron to make the connection.</t>
+  </si>
+  <si>
+    <t>It was a LOT easier with these right tools.</t>
+  </si>
+  <si>
+    <t>I tested the ESP32 and it's still working. The 5V and 3v3 rails work correctly too. The supercapacitor takes around 45 seconds to fully charge and keeps the device awake for over 15 seconds!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I may </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">change the supercapacitor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as the circuit only needs to be alive for around 1 second. Lower capacitance also means it will charge faster and reduce chance of losing video clip at start of boot up.</t>
+    </r>
+  </si>
+  <si>
+    <t>Next steps are to program the ESP32 and check if the camera can be detected and if it can take pictures. Following that, I will test the IO expander and subsequently the LEDs and buttons.</t>
   </si>
 </sst>
 </file>
@@ -7414,10 +7461,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
-  <dimension ref="A2:D239"/>
+  <dimension ref="A2:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A218" sqref="A218"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A254" sqref="A254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8083,6 +8130,51 @@
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" s="59">
+        <v>44430</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" s="39" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move old production stuff to new folder. start pcb spin 2: add test points (smd and pads). add third diode as currently disconnected USB can not be detected. increase LED resistor values are too bright. improve OLED footprint (to accomodate inaccuracies in drawing).
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71648E89-6A48-4144-ACE2-8142B8E37676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94336B9-91C8-48CB-BCF5-CD828C250A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Outline" sheetId="7" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="284">
   <si>
     <t>Risk</t>
   </si>
@@ -889,9 +889,6 @@
     <t>Buy more OLEDs, as they take a while to deliver</t>
   </si>
   <si>
-    <t>Check other components that we may need now that some of them were using during soldering</t>
-  </si>
-  <si>
     <t>Buy twice as many as components needed, accidents happen more often than I thought they would</t>
   </si>
   <si>
@@ -946,6 +943,72 @@
   </si>
   <si>
     <t>Next steps are to program the ESP32 and check if the camera can be detected and if it can take pictures. Following that, I will test the IO expander and subsequently the LEDs and buttons.</t>
+  </si>
+  <si>
+    <t>Check other components that we may need now that some of them were used during soldering</t>
+  </si>
+  <si>
+    <t>Today I will be modifying the PCB to make it easier to debug issues and build the firmware for the device.</t>
+  </si>
+  <si>
+    <t>2. Give space around mounting holes</t>
+  </si>
+  <si>
+    <t>3. Flip SD card</t>
+  </si>
+  <si>
+    <t>4. Footprint of buttons</t>
+  </si>
+  <si>
+    <t>5. Min via size to 0.45 mm</t>
+  </si>
+  <si>
+    <t>6. Silk screen for UART connector</t>
+  </si>
+  <si>
+    <t>7. Increase LED resistor value</t>
+  </si>
+  <si>
+    <t>8. Move FFC connector inwards</t>
+  </si>
+  <si>
+    <t>9. Put FFC connector on other side? I.e. swap with the uart connector</t>
+  </si>
+  <si>
+    <t>10. On/off switch to power off supercap for when developing, or do somethign w/reset button</t>
+  </si>
+  <si>
+    <t>11. LDO gets too hot. add vias, and leave spacing</t>
+  </si>
+  <si>
+    <t>QOL:</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>1. Change FFC connector for the board-board FFC</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>For end product</t>
+  </si>
+  <si>
+    <t>12. Add test points</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>13. Impove footprint of OLED (the pads are too short)</t>
+  </si>
+  <si>
+    <t>Removing these:</t>
   </si>
 </sst>
 </file>
@@ -2224,6 +2287,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>503863</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>3287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C90AF249-3DF3-43D8-949C-33504B2317D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="47244000"/>
+          <a:ext cx="7695238" cy="4184762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7461,10 +7568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
-  <dimension ref="A2:D255"/>
+  <dimension ref="A2:P275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A254" sqref="A254"/>
+    <sheetView tabSelected="1" topLeftCell="A252" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F282" sqref="F282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8057,12 +8164,12 @@
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8114,12 +8221,12 @@
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
@@ -8139,42 +8246,154 @@
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>261</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A257" s="59">
+        <v>44437</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>263</v>
+      </c>
+      <c r="P259" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A261" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C261" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>281</v>
+      </c>
+      <c r="B262" t="s">
+        <v>279</v>
+      </c>
+      <c r="C262" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>278</v>
+      </c>
+      <c r="B263" t="s">
+        <v>279</v>
+      </c>
+      <c r="C263" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C264" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>281</v>
+      </c>
+      <c r="C265" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C266" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C267" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="268" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>281</v>
+      </c>
+      <c r="C268" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C269" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C270" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C271" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="272" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C272" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="273" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C273" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="274" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C274" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="275" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B275" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make board on breadboard for easier debugging and fixing. will start writing f/w on this board
</commit_message>
<xml_diff>
--- a/project_plan/Project_planning.xlsx
+++ b/project_plan/Project_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94336B9-91C8-48CB-BCF5-CD828C250A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA15CDDD-AE3E-45E0-9560-0384868B7FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7F1CE0F2-BD3C-42CE-8FA6-BDD773462733}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Outline" sheetId="7" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="296">
   <si>
     <t>Risk</t>
   </si>
@@ -981,9 +981,6 @@
     <t>11. LDO gets too hot. add vias, and leave spacing</t>
   </si>
   <si>
-    <t>QOL:</t>
-  </si>
-  <si>
     <t>Done?</t>
   </si>
   <si>
@@ -1009,6 +1006,57 @@
   </si>
   <si>
     <t>Removing these:</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>NOT USING</t>
+  </si>
+  <si>
+    <t>Added 3 LEDs, for 5V (USB), 5V (supercap) and 3V3 for visual debugging</t>
+  </si>
+  <si>
+    <t>Tested power and all rails seem to be working correctly.</t>
+  </si>
+  <si>
+    <t>If USB is disconnected, the RED LED turns off, GREEN LED and YELLOW led are on</t>
+  </si>
+  <si>
+    <t>which means USB connection can be detected by MCU.</t>
+  </si>
+  <si>
+    <t>The MCU stays on until the voltage drops below X (need to measure) and</t>
+  </si>
+  <si>
+    <t>after this the MCU keeps trying to restart.</t>
+  </si>
+  <si>
+    <t>Camera seems to be working using the example code from esp-idf.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Next time: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test OLED screen (example) and finally GPIO expander example</t>
+    </r>
+  </si>
+  <si>
+    <t>After this, start the firmware architecture and start writing the f/w.</t>
+  </si>
+  <si>
+    <t>Decided to build circuit on breadboard. The PCBA (spin 1) UART becomes unreadable after a while and there aren't enough test points to understand what the issue is.</t>
+  </si>
+  <si>
+    <t>This will allow me to test the hardware, make changes easily, and start developing the firmware. If FW can't be developed due to h/w limitations, I will design another board. Otherwise I will finish f/w first.</t>
   </si>
 </sst>
 </file>
@@ -2331,6 +2379,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>175005</xdr:colOff>
+      <xdr:row>317</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D3EC8A-3A3E-4C4C-B94C-AF9FF0396D8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5539741" y="53484781"/>
+          <a:ext cx="3451604" cy="4564380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7568,10 +7660,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9BFAE4-050E-4068-9513-EE9898A0E724}">
-  <dimension ref="A2:P275"/>
+  <dimension ref="A2:P310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F282" sqref="F282"/>
+    <sheetView tabSelected="1" topLeftCell="A283" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A292" sqref="A292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8294,50 +8386,53 @@
         <v>263</v>
       </c>
       <c r="P259" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A261" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B261" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="262" spans="1:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B262" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C262" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
+        <v>277</v>
+      </c>
+      <c r="B263" t="s">
         <v>278</v>
-      </c>
-      <c r="B263" t="s">
-        <v>279</v>
       </c>
       <c r="C263" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>280</v>
+      </c>
       <c r="C264" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C265" t="s">
         <v>266</v>
@@ -8355,18 +8450,30 @@
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C268" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>283</v>
+      </c>
+      <c r="B269" t="s">
+        <v>284</v>
+      </c>
       <c r="C269" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>283</v>
+      </c>
+      <c r="B270" t="s">
+        <v>284</v>
+      </c>
       <c r="C270" t="s">
         <v>271</v>
       </c>
@@ -8381,20 +8488,92 @@
         <v>273</v>
       </c>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>280</v>
+      </c>
       <c r="C273" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C274" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B275" t="s">
-        <v>274</v>
-      </c>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A286" s="59">
+        <v>44438</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A289" s="39" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>285</v>
+      </c>
+      <c r="B293" s="5"/>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A294" s="5"/>
+      <c r="B294" s="5"/>
+      <c r="C294" s="5"/>
+      <c r="D294" s="5"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>286</v>
+      </c>
+      <c r="D295" s="39"/>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>